<commit_message>
13-08: Tim hieu load balancer, api gateway, storage, ve mau topo
</commit_message>
<xml_diff>
--- a/VDT GPDĐ.xlsx
+++ b/VDT GPDĐ.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Job\1. Phong Di Dong\VDT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Học tập\VDT\GD2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71C902F-CF0A-4843-B873-278C9590C409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15490" windowHeight="6890" activeTab="1"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,7 +261,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -630,22 +631,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="7" width="25.08984375" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" customWidth="1"/>
-    <col min="9" max="9" width="19.6328125" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -674,7 +675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="126" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="134.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -703,7 +704,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="288" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="76.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -732,7 +733,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -765,21 +766,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.26953125" customWidth="1"/>
-    <col min="3" max="3" width="82.54296875" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="82.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -793,7 +794,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="112" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -807,7 +808,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="84" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
@@ -821,7 +822,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="84" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -835,7 +836,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>38</v>
       </c>
@@ -849,7 +850,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="98" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -863,7 +864,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>43</v>
       </c>
@@ -877,7 +878,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="56" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>46</v>
       </c>

</xml_diff>